<commit_message>
Update the doc and add mac check feature
</commit_message>
<xml_diff>
--- a/doc/基站广播包内容说明.xlsx
+++ b/doc/基站广播包内容说明.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>01</t>
   </si>
@@ -253,6 +253,10 @@
 DE AD 03 01 03 BE EF
 &gt;&gt;0xDE 0xAD 0x08 0x00 0x0D 0x00 0x0F 0x00 0xC8 0xFD 0x19 0x9C 0xD6 0x54 0xBE 0xEF
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stationIndex，暂定每分钟增长1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -400,7 +404,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -410,43 +414,46 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -735,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4:Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -749,87 +756,89 @@
     <col min="21" max="21" width="37.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="29.26953125" style="1" customWidth="1"/>
     <col min="23" max="23" width="24.6328125" style="1" customWidth="1"/>
-    <col min="24" max="30" width="3.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.54296875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="15.453125" style="1" customWidth="1"/>
+    <col min="26" max="30" width="3.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AD1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
     </row>
     <row r="2" spans="1:30" ht="14.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="5" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="8"/>
-      <c r="X2" s="7" t="s">
+      <c r="W2" s="13"/>
+      <c r="X2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -933,69 +942,73 @@
       <c r="U4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="V4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="W4" s="10"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y4" s="16"/>
     </row>
     <row r="6" spans="1:30" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
-    </row>
-    <row r="7" spans="1:30" ht="84" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+    </row>
+    <row r="7" spans="1:30" ht="56" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="14" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="V7" s="14"/>
+      <c r="V7" s="9"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1010,24 +1023,24 @@
       <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
       <c r="U8" s="1" t="s">
         <v>35</v>
       </c>
@@ -1056,547 +1069,548 @@
       </c>
     </row>
     <row r="14" spans="1:30" ht="14" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
-      <c r="T31" s="15"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
-      <c r="T32" s="15"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
-      <c r="T33" s="15"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
-      <c r="T34" s="15"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
-      <c r="T35" s="15"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X2:AD2"/>
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="X4:Y4"/>
     <mergeCell ref="A6:U6"/>
     <mergeCell ref="E8:T8"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="U7:V7"/>
     <mergeCell ref="A14:T37"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X2:AD2"/>
-    <mergeCell ref="A1:AD1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix the changing adv data issue.
</commit_message>
<xml_diff>
--- a/doc/基站广播包内容说明.xlsx
+++ b/doc/基站广播包内容说明.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>01</t>
   </si>
@@ -179,14 +179,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>02 01 06 1A FF 4C 00 02 15 53 4D 54 12 13 14 15 16 02 01 02 20 00 0A 23 24 FF FF FF FF CD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -215,36 +207,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>02，更新广播包内容</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>03，更新广播包发送间隔（单位100ms）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>04，获取当前配置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>01，基站角色切换</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Example
-//让基站进入发送广播角色
-DE AD 00 01 01 BE EF
-//更改基站发送广播的内容
-DE AD 01 1E 02 01 06 1A FF 4C 00 02 15 53 4D 54 12 13 14 15 16 17 18 19 20 21 22 23 24 FF FF FF FF CD BE EF
-// Change Interval to 500ms
-DE AD 02 01 05 BE EF
-// 获取当前基站角色
-DE AD 03 01 00 BE EF
-&gt;&gt;0xDE 0xAD 0x01 0xBE 0xEF
-// 获取当前基站MAC
-DE AD 03 01 03 BE EF
-&gt;&gt;0xDE 0xAD 0x08 0x00 0x0D 0x00 0x0F 0x00 0xC8 0xFD 0x19 0x9C 0xD6 0x54 0xBE 0xEF
-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -356,6 +319,36 @@
   </si>
   <si>
     <t>秒数是 ((Z2 &lt;&lt; 8) + Z1)，单位100毫秒，16进制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>03，获取当前配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>02，更新广播间隔（100ms单位）以及包内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>02 02 01 06 1A FF 4C 00 02 15 53 4D 54 12 13 14 15 16 02 01 02 20 00 0A 23 24 FF FF FF FF CD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Example
+//让基站进入发送广播角色
+DE AD 00 01 01 BE EF
+//闪灯命令+200ms发送间隔
+DE AD 01 1F 02 02 01 06 1A FF 4C 00 02 15 53 4D 54 C1 13 14 15 16 02 03 FF 20 00 3C 23 24 00 00 00 00 CD BE EF
+//更改基站发送广播的内容+200ms发送间隔
+DE AD 01 1F 02 02 01 06 1A FF 4C 00 02 15 53 4D 54 12 13 14 15 16 17 18 19 20 21 22 23 24 FF FF FF FF CD BE EF
+// 获取当前基站状态
+DE AD 02 00 BE EF
+&gt;&gt;DE AD 01 02 8C AD 3F 7F C7 F0 02 01 06 1A 3F 4C 02 15 53 4D 54 3F 13 14 15 16 02 03 3F 20 3C 23 24 CD BE EF
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -850,15 +843,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5:X5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:U43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="3.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.36328125" style="1" customWidth="1"/>
     <col min="5" max="13" width="3.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.54296875" style="1" customWidth="1"/>
     <col min="15" max="19" width="3.1796875" style="1" bestFit="1" customWidth="1"/>
@@ -953,43 +946,43 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>11</v>
@@ -1007,22 +1000,22 @@
         <v>14</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>17</v>
@@ -1031,24 +1024,24 @@
         <v>18</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="AC3" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AD3" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="AE3" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -1143,13 +1136,13 @@
     </row>
     <row r="5" spans="1:31" ht="70" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N5" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="N5" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="T5" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>22</v>
@@ -1158,15 +1151,15 @@
         <v>22</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="X5" s="18"/>
       <c r="Y5" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="Z5" s="10"/>
       <c r="AA5" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="AB5" s="10"/>
       <c r="AC5" s="10"/>
@@ -1175,13 +1168,13 @@
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="N6" s="7"/>
       <c r="T6" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="V6" s="14" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="W6" s="14"/>
       <c r="X6" s="14"/>
@@ -1230,17 +1223,17 @@
     </row>
     <row r="13" spans="1:31" ht="56" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -1258,7 +1251,7 @@
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
       <c r="V13" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="W13" s="13"/>
     </row>
@@ -1273,10 +1266,10 @@
         <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -1294,35 +1287,30 @@
       <c r="T14" s="11"/>
       <c r="U14" s="11"/>
       <c r="V14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D18" s="1" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="2:21" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>

</xml_diff>